<commit_message>
A few more excel tweaks, tests, COM cleanup
</commit_message>
<xml_diff>
--- a/test/good_dyns/excel/tests.xlsx
+++ b/test/good_dyns/excel/tests.xlsx
@@ -17,12 +17,18 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
     <t>a</t>
   </si>
   <si>
     <t>s</t>
+  </si>
+  <si>
+    <t>Domingo</t>
+  </si>
+  <si>
+    <t>Pedro</t>
   </si>
 </sst>
 </file>
@@ -361,7 +367,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D1"/>
+  <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="D3" sqref="D3"/>
@@ -381,6 +387,14 @@
       </c>
       <c r="D1" t="s">
         <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C4" t="s">
+        <v>2</v>
+      </c>
+      <c r="D4" t="s">
+        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>